<commit_message>
Se modifica el CP
</commit_message>
<xml_diff>
--- a/Registrar.xlsx
+++ b/Registrar.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbecauich/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeridaSoft\Desktop\CP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9CDEBCE-2C18-E144-B9CE-5443978A2DE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Registrar-CP001" sheetId="2" r:id="rId2"/>
-    <sheet name="Registrar-CP003" sheetId="5" r:id="rId3"/>
-    <sheet name="Registrar-CP002" sheetId="4" r:id="rId4"/>
+    <sheet name="CU001-CP001" sheetId="2" r:id="rId2"/>
+    <sheet name="CU001-CP002" sheetId="4" r:id="rId3"/>
+    <sheet name="CU001-CP003" sheetId="5" r:id="rId4"/>
+    <sheet name="CU001-CP004" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
   <si>
     <t>Tipo de dato</t>
   </si>
@@ -126,9 +126,6 @@
     <t>FND</t>
   </si>
   <si>
-    <t>Registrar</t>
-  </si>
-  <si>
     <t>CP para probar la funcionalidad del registro</t>
   </si>
   <si>
@@ -139,10 +136,6 @@
   </si>
   <si>
     <t>CP.001.FP.Registar</t>
-  </si>
-  <si>
-    <t>Se debe tener instalada la aplicaciòn
-Se debe ingresar el CURP</t>
   </si>
   <si>
     <t>Acceder a la aplicación</t>
@@ -155,9 +148,6 @@
       * Registrar</t>
   </si>
   <si>
-    <t>Presionar el botòn "Registrar"</t>
-  </si>
-  <si>
     <t>Se muestra pantalla con los siguientes campos:
  * CURP
  * Botón
@@ -170,24 +160,10 @@
     <t>Se muestra mensaje "Cargando, espere por favor"</t>
   </si>
   <si>
-    <t>Se muestra mensaje "Cargando, espere por favor", se carga pantalla para la carga de datos persanales</t>
-  </si>
-  <si>
-    <t>CP.001.FP.Curp.incorrecto</t>
-  </si>
-  <si>
-    <t>Se debe tener instalada la aplicaciòn
-El curP es incorrecto
-Se debe ejecutar el CP001.FP hasta el paso 2</t>
-  </si>
-  <si>
     <t>Se consume el servicio para validar el curp</t>
   </si>
   <si>
     <t>Se muestra en pantalla mensaje "Curp Incorrecto, corrija e intente de nuevo"</t>
-  </si>
-  <si>
-    <t>CP.001.FP.Curp.vacio</t>
   </si>
   <si>
     <t>Se debe tener instalada la aplicación
@@ -198,12 +174,54 @@
   </si>
   <si>
     <t>El campo CURP se marca de rojo y muestra mensaje "Campo requerido"</t>
+  </si>
+  <si>
+    <t>Presionar el botón "Registrar"</t>
+  </si>
+  <si>
+    <t>CP.002.FA.Curp.incorrecto</t>
+  </si>
+  <si>
+    <t>CP.001.FA.Curp.vacio</t>
+  </si>
+  <si>
+    <t>CU001 - Registrar</t>
+  </si>
+  <si>
+    <t>Se debe tener instalada la aplicación
+El curp es incorrecto
+Se debe ejecutar el CP001.FP hasta el paso 2</t>
+  </si>
+  <si>
+    <t>Se debe tener instalada la aplicación
+Se debe ingresar el CURP</t>
+  </si>
+  <si>
+    <t>Capturar el CURP</t>
+  </si>
+  <si>
+    <t>Se desmarca el campo y se oculta el mensaje "Campo requerido".</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje "Cargando, espere por favor", se carga pantalla para la carga de datos personales</t>
+  </si>
+  <si>
+    <t>CP.004.FA.Sin conexión</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje "Sin conexión a la red, intente de nuevo."</t>
+  </si>
+  <si>
+    <t>Se debe tener instalada la aplicación
+Se debe ingresar el CURP
+Los servicios web del SAP deben estar disponibles.
+No se tiene conexión a la red y/o BD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -430,6 +448,51 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -439,32 +502,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -474,21 +513,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -545,7 +569,7 @@
         <xdr:cNvPr id="2" name="Imagen 1" descr="https://lh3.googleusercontent.com/zAUUpAdaWJaQ_jYK8NqAAgEOs_LZOhAP3cYWxEh9_VVCDmHhrSPUwxDs3y1r6RWH6r0z=s170">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -611,7 +635,7 @@
         <xdr:cNvPr id="2" name="Imagen 1" descr="https://lh3.googleusercontent.com/zAUUpAdaWJaQ_jYK8NqAAgEOs_LZOhAP3cYWxEh9_VVCDmHhrSPUwxDs3y1r6RWH6r0z=s170">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -677,7 +701,7 @@
         <xdr:cNvPr id="2" name="Imagen 1" descr="https://lh3.googleusercontent.com/zAUUpAdaWJaQ_jYK8NqAAgEOs_LZOhAP3cYWxEh9_VVCDmHhrSPUwxDs3y1r6RWH6r0z=s170">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1332DB0B-586C-2349-9248-9C9C176F9AC4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E123EB7A-22CF-FE48-B062-ACA38C834787}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -743,7 +767,7 @@
         <xdr:cNvPr id="2" name="Imagen 1" descr="https://lh3.googleusercontent.com/zAUUpAdaWJaQ_jYK8NqAAgEOs_LZOhAP3cYWxEh9_VVCDmHhrSPUwxDs3y1r6RWH6r0z=s170">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E123EB7A-22CF-FE48-B062-ACA38C834787}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1332DB0B-586C-2349-9248-9C9C176F9AC4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -768,6 +792,72 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="1786160" cy="923925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>135160</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>733425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1" descr="https://lh3.googleusercontent.com/zAUUpAdaWJaQ_jYK8NqAAgEOs_LZOhAP3cYWxEh9_VVCDmHhrSPUwxDs3y1r6RWH6r0z=s170">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1659160" cy="923925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1051,143 +1141,143 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F7" sqref="F7:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="19" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="1" spans="1:17" s="21" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="32" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
       <c r="Q2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20"/>
       <c r="Q3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
       <c r="Q4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="24"/>
-    </row>
-    <row r="6" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="35">
-        <v>43885</v>
-      </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24"/>
-    </row>
-    <row r="7" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="27">
+        <v>43887</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
-    </row>
-    <row r="8" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="1" t="str">
-        <f>IF('Registrar-CP001'!C2:H2="","",'Registrar-CP001'!C2:H2)</f>
+        <f>IF('CU001-CP001'!C2:H2="","",'CU001-CP001'!C2:H2)</f>
         <v/>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22" t="str">
-        <f>IF('Registrar-CP001'!F2:H2="","",'Registrar-CP001'!F2:H2)</f>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24" t="str">
+        <f>IF('CU001-CP001'!F2:H2="","",'CU001-CP001'!F2:H2)</f>
         <v/>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="24"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>23</v>
       </c>
@@ -1201,8 +1291,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <f>F6</f>
+        <v>43887</v>
+      </c>
       <c r="B12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1211,19 +1304,19 @@
       </c>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="A8:B8"/>
@@ -1252,232 +1345,232 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:H16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.5" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:8" s="19" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+    <row r="1" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:8" s="21" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
       <c r="E4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="5" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="26"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="29"/>
+      <c r="C5" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="25" t="s">
+      <c r="C7" s="29"/>
+      <c r="D7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="26"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="73" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="72.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
+      <c r="B8" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="91" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="90.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>2</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
+      <c r="B9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>3</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
+      <c r="B10" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="26"/>
-    </row>
-    <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="29"/>
+      <c r="C12" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="25" t="s">
+      <c r="D12" s="29"/>
+      <c r="E12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="25" t="s">
+      <c r="F12" s="29"/>
+      <c r="G12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="26"/>
-    </row>
-    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="24"/>
-    </row>
-    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="24"/>
-    </row>
-    <row r="17" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-    </row>
-    <row r="18" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="H12" s="29"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="30" t="s">
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="30"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
@@ -1532,7 +1625,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Data!$Q$2:$Q$4</xm:f>
           </x14:formula1>
@@ -1545,473 +1638,216 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDA94A3-1E51-4644-81B5-EDCC666CE8BC}">
-  <dimension ref="A1:H16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.5" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:8" s="19" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+    <row r="1" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:8" s="21" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
       <c r="E4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="5" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="16" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="26"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="25" t="s">
+      <c r="C7" s="29"/>
+      <c r="D7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="26"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>1</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="B8" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
-    </row>
-    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="26"/>
-    </row>
-    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="24"/>
-    </row>
-    <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="24"/>
-    </row>
-    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-    </row>
-    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="30"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="A1:XFD2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:H5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4865765-2D75-7E4A-8389-5D5650E387F2}">
-          <x14:formula1>
-            <xm:f>Data!$Q$2:$Q$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>E16:F16</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF35CDB-C866-BC40-BA67-F7AFE8DD194E}">
-  <dimension ref="A1:H17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="37.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.5" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
-    <col min="8" max="8" width="34" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:8" s="19" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="5" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="26"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>1</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:8" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>2</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="39"/>
+      <c r="B9" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="41"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
+      <c r="E9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="25" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="25" t="s">
+      <c r="D11" s="29"/>
+      <c r="E11" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="25" t="s">
+      <c r="F11" s="29"/>
+      <c r="G11" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="26"/>
-    </row>
-    <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="24"/>
-    </row>
-    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="24"/>
-    </row>
-    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-    </row>
-    <row r="17" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="30" t="s">
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="30"/>
+      <c r="F17" s="37"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
@@ -2064,7 +1900,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4E6FF25-5449-6C42-BE38-FB857FB2C685}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Data!$Q$2:$Q$4</xm:f>
           </x14:formula1>
@@ -2074,4 +1910,572 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:8" s="21" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>1</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>2</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="29"/>
+      <c r="C11" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="37"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="41">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A1:XFD2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$Q$2:$Q$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E17:F17</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:8" s="21" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="72.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="90.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>3</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="29"/>
+      <c r="G12" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="29"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="43">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="A1:XFD2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="E18:F18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$Q$2:$Q$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E18:F18</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>